<commit_message>
Sprint 1 Week 2 Deliverable
</commit_message>
<xml_diff>
--- a/bookkeeping/sprint1/overview/s1_burndown.xlsx
+++ b/bookkeeping/sprint1/overview/s1_burndown.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>ideal</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Team McBuddy</t>
+  </si>
+  <si>
+    <t>Phil</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -129,9 +135,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -294,67 +301,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>105.0</c:v>
+                  <c:v>119.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.0</c:v>
+                  <c:v>113.333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>95.0</c:v>
+                  <c:v>107.666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.0</c:v>
+                  <c:v>101.999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>85.0</c:v>
+                  <c:v>96.333333332</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80.0</c:v>
+                  <c:v>90.666666665</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>75.0</c:v>
+                  <c:v>84.999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70.0</c:v>
+                  <c:v>79.33333333100001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>65.0</c:v>
+                  <c:v>73.666666664</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>60.0</c:v>
+                  <c:v>67.999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>55.0</c:v>
+                  <c:v>62.33333333</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>50.0</c:v>
+                  <c:v>56.666666663</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>45.0</c:v>
+                  <c:v>50.999999996</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>40.0</c:v>
+                  <c:v>45.333333329</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>35.0</c:v>
+                  <c:v>39.666666662</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>30.0</c:v>
+                  <c:v>33.999999995</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>25.0</c:v>
+                  <c:v>28.333333328</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>20.0</c:v>
+                  <c:v>22.666666661</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>15.0</c:v>
+                  <c:v>16.999999994</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10.0</c:v>
+                  <c:v>11.333333327</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.0</c:v>
+                  <c:v>5.66666666</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>0.0</c:v>
@@ -463,28 +470,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>105.0</c:v>
+                  <c:v>119.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>103.0</c:v>
+                  <c:v>117.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>103.0</c:v>
+                  <c:v>117.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>103.0</c:v>
+                  <c:v>117.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>98.0</c:v>
+                  <c:v>112.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90.0</c:v>
+                  <c:v>104.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>85.0</c:v>
+                  <c:v>99.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>97.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>89.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>83.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>83.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>83.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>82.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>79.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>78.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -501,11 +529,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2066841016"/>
-        <c:axId val="2065942968"/>
+        <c:axId val="2107908680"/>
+        <c:axId val="2107901000"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2066841016"/>
+        <c:axId val="2107908680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -539,14 +567,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2065942968"/>
+        <c:crossAx val="2107901000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2065942968"/>
+        <c:axId val="2107901000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -576,7 +604,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066841016"/>
+        <c:crossAx val="2107908680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -610,7 +638,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -955,10 +983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W27"/>
+  <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1040,68 +1068,68 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>105</v>
+      <c r="B3" s="2">
+        <v>119</v>
       </c>
       <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3">
-        <v>95</v>
+        <v>113.333333333</v>
+      </c>
+      <c r="D3" s="2">
+        <v>107.666666666</v>
       </c>
       <c r="E3">
-        <v>90</v>
-      </c>
-      <c r="F3">
-        <v>85</v>
+        <v>101.999999999</v>
+      </c>
+      <c r="F3" s="2">
+        <v>96.333333331999995</v>
       </c>
       <c r="G3">
-        <v>80</v>
-      </c>
-      <c r="H3">
-        <v>75</v>
+        <v>90.666666664999994</v>
+      </c>
+      <c r="H3" s="2">
+        <v>84.999999998000007</v>
       </c>
       <c r="I3">
-        <v>70</v>
-      </c>
-      <c r="J3">
-        <v>65</v>
+        <v>79.333333331000006</v>
+      </c>
+      <c r="J3" s="2">
+        <v>73.666666664000005</v>
       </c>
       <c r="K3">
-        <v>60</v>
-      </c>
-      <c r="L3">
-        <v>55</v>
+        <v>67.999999997000003</v>
+      </c>
+      <c r="L3" s="2">
+        <v>62.333333330000002</v>
       </c>
       <c r="M3">
-        <v>50</v>
-      </c>
-      <c r="N3">
-        <v>45</v>
+        <v>56.666666663000001</v>
+      </c>
+      <c r="N3" s="2">
+        <v>50.999999996</v>
       </c>
       <c r="O3">
-        <v>40</v>
-      </c>
-      <c r="P3">
-        <v>35</v>
+        <v>45.333333328999998</v>
+      </c>
+      <c r="P3" s="2">
+        <v>39.666666661999997</v>
       </c>
       <c r="Q3">
-        <v>30</v>
-      </c>
-      <c r="R3">
-        <v>25</v>
+        <v>33.999999995000003</v>
+      </c>
+      <c r="R3" s="2">
+        <v>28.333333327999998</v>
       </c>
       <c r="S3">
-        <v>20</v>
-      </c>
-      <c r="T3">
-        <v>15</v>
+        <v>22.666666661000001</v>
+      </c>
+      <c r="T3" s="2">
+        <v>16.999999994</v>
       </c>
       <c r="U3">
-        <v>10</v>
-      </c>
-      <c r="V3">
-        <v>5</v>
+        <v>11.333333327</v>
+      </c>
+      <c r="V3" s="2">
+        <v>5.6666666599999997</v>
       </c>
       <c r="W3">
         <v>0</v>
@@ -1112,28 +1140,49 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="C4">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="D4">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="E4">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="F4">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="G4">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="H4">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="I4">
+        <v>97</v>
+      </c>
+      <c r="J4">
+        <v>89</v>
+      </c>
+      <c r="K4">
         <v>83</v>
+      </c>
+      <c r="L4">
+        <v>83</v>
+      </c>
+      <c r="M4">
+        <v>83</v>
+      </c>
+      <c r="N4">
+        <v>82</v>
+      </c>
+      <c r="O4">
+        <v>79</v>
+      </c>
+      <c r="P4">
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -1161,6 +1210,32 @@
       <c r="H6">
         <v>2</v>
       </c>
+      <c r="I6">
+        <v>8</v>
+      </c>
+      <c r="J6">
+        <v>6</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="N8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:23">
       <c r="C9" t="s">
@@ -1197,6 +1272,9 @@
       <c r="C11">
         <v>5</v>
       </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
@@ -1208,6 +1286,9 @@
       <c r="C12">
         <v>0</v>
       </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
       <c r="P12" t="s">
         <v>12</v>
       </c>
@@ -1222,6 +1303,9 @@
       <c r="C13">
         <v>0</v>
       </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
       <c r="P13" t="s">
         <v>13</v>
       </c>
@@ -1236,6 +1320,9 @@
       <c r="C14">
         <v>7</v>
       </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
       <c r="P14" t="s">
         <v>24</v>
       </c>
@@ -1250,60 +1337,90 @@
       <c r="C15">
         <v>0</v>
       </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:23">
       <c r="A16" t="s">
         <v>9</v>
       </c>
       <c r="B16">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>24</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
+      <c r="D18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>7</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>11</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
         <v>11</v>
       </c>
-      <c r="B19">
-        <f>SUM(B11:B18)</f>
-        <v>105</v>
-      </c>
-      <c r="C19">
-        <f>SUM(C11:C18)</f>
+      <c r="B20">
+        <f>SUM(B11:B19)</f>
+        <v>119</v>
+      </c>
+      <c r="C20">
+        <f>SUM(C11:C19)</f>
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
+      <c r="D20">
+        <f>SUM(D11:D19)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correct burndown up to 03 Feb
</commit_message>
<xml_diff>
--- a/bookkeeping/sprint1/overview/s1_burndown.xlsx
+++ b/bookkeeping/sprint1/overview/s1_burndown.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>ideal</t>
   </si>
@@ -85,12 +85,6 @@
   </si>
   <si>
     <t>sprint 1</t>
-  </si>
-  <si>
-    <t>TODO:</t>
-  </si>
-  <si>
-    <t>convert real entries to day before minus finished</t>
   </si>
   <si>
     <t>Team McBuddy</t>
@@ -509,10 +503,16 @@
                   <c:v>82.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>79.0</c:v>
+                  <c:v>73.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>78.0</c:v>
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -529,11 +529,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2107908680"/>
-        <c:axId val="2107901000"/>
+        <c:axId val="2125188456"/>
+        <c:axId val="2125192552"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2107908680"/>
+        <c:axId val="2125188456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -567,14 +567,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107901000"/>
+        <c:crossAx val="2125192552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2107901000"/>
+        <c:axId val="2125192552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -604,7 +604,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107908680"/>
+        <c:crossAx val="2125188456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -983,10 +983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W28"/>
+  <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1179,10 +1179,16 @@
         <v>82</v>
       </c>
       <c r="O4">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="P4">
-        <v>78</v>
+        <v>70</v>
+      </c>
+      <c r="Q4">
+        <v>64</v>
+      </c>
+      <c r="R4">
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -1226,15 +1232,21 @@
         <v>1</v>
       </c>
       <c r="N6">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="O6">
         <v>3</v>
       </c>
+      <c r="P6">
+        <v>6</v>
+      </c>
+      <c r="Q6">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:23">
       <c r="N8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:23">
@@ -1272,9 +1284,6 @@
       <c r="C11">
         <v>5</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
@@ -1286,9 +1295,6 @@
       <c r="C12">
         <v>0</v>
       </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
       <c r="P12" t="s">
         <v>12</v>
       </c>
@@ -1303,9 +1309,6 @@
       <c r="C13">
         <v>0</v>
       </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
       <c r="P13" t="s">
         <v>13</v>
       </c>
@@ -1320,11 +1323,8 @@
       <c r="C14">
         <v>7</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
       <c r="P14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:23">
@@ -1337,9 +1337,6 @@
       <c r="C15">
         <v>0</v>
       </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
     </row>
     <row r="16" spans="1:23">
       <c r="A16" t="s">
@@ -1351,13 +1348,10 @@
       <c r="C16">
         <v>0</v>
       </c>
-      <c r="D16">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17">
         <v>11</v>
@@ -1365,11 +1359,8 @@
       <c r="C17">
         <v>0</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1379,11 +1370,8 @@
       <c r="C18">
         <v>10</v>
       </c>
-      <c r="D18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1393,11 +1381,8 @@
       <c r="C19">
         <v>0</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1408,20 +1393,6 @@
       <c r="C20">
         <f>SUM(C11:C19)</f>
         <v>22</v>
-      </c>
-      <c r="D20">
-        <f>SUM(D11:D19)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update tasks formatting,  SMT7
Update actual-hours chart and meetings time, correct burndown errors,
update burndown to 05 February before end-of-sprint meeting
</commit_message>
<xml_diff>
--- a/bookkeeping/sprint1/overview/s1_burndown.xlsx
+++ b/bookkeeping/sprint1/overview/s1_burndown.xlsx
@@ -512,7 +512,16 @@
                   <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>46.0</c:v>
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>36.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -529,11 +538,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2125188456"/>
-        <c:axId val="2125192552"/>
+        <c:axId val="2082587272"/>
+        <c:axId val="2082582504"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2125188456"/>
+        <c:axId val="2082587272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -567,14 +576,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125192552"/>
+        <c:crossAx val="2082582504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2125192552"/>
+        <c:axId val="2082582504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -604,7 +613,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125188456"/>
+        <c:crossAx val="2082587272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -986,7 +995,7 @@
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1188,7 +1197,16 @@
         <v>64</v>
       </c>
       <c r="R4">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="S4">
+        <v>42</v>
+      </c>
+      <c r="T4">
+        <v>38</v>
+      </c>
+      <c r="U4">
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -1241,7 +1259,16 @@
         <v>6</v>
       </c>
       <c r="Q6">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>4</v>
+      </c>
+      <c r="T6">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:23">
@@ -1284,6 +1311,16 @@
       <c r="C11">
         <v>5</v>
       </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <f>SUM(C11,D11,E11)</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
@@ -1295,6 +1332,16 @@
       <c r="C12">
         <v>0</v>
       </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:F19" si="0">SUM(C12,D12,E12)</f>
+        <v>13</v>
+      </c>
       <c r="P12" t="s">
         <v>12</v>
       </c>
@@ -1309,6 +1356,16 @@
       <c r="C13">
         <v>0</v>
       </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="P13" t="s">
         <v>13</v>
       </c>
@@ -1323,6 +1380,16 @@
       <c r="C14">
         <v>7</v>
       </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="P14" t="s">
         <v>22</v>
       </c>
@@ -1337,6 +1404,16 @@
       <c r="C15">
         <v>0</v>
       </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:23">
       <c r="A16" t="s">
@@ -1348,8 +1425,18 @@
       <c r="C16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1359,8 +1446,18 @@
       <c r="C17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1370,8 +1467,18 @@
       <c r="C18">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1381,8 +1488,18 @@
       <c r="C19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1393,6 +1510,18 @@
       <c r="C20">
         <f>SUM(C11:C19)</f>
         <v>22</v>
+      </c>
+      <c r="D20">
+        <f>SUM(D11:D19)</f>
+        <v>36</v>
+      </c>
+      <c r="E20">
+        <f>SUM(E11:E19)</f>
+        <v>26</v>
+      </c>
+      <c r="F20">
+        <f>SUM(F11:F19)</f>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1400,6 +1529,7 @@
     <sortCondition ref="A11"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Update burndown for sprint end meeting
</commit_message>
<xml_diff>
--- a/bookkeeping/sprint1/overview/s1_burndown.xlsx
+++ b/bookkeeping/sprint1/overview/s1_burndown.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="21060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -515,13 +515,13 @@
                   <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>42.0</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>38.0</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>36.0</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -538,11 +538,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2082587272"/>
-        <c:axId val="2082582504"/>
+        <c:axId val="2083419960"/>
+        <c:axId val="2084307560"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2082587272"/>
+        <c:axId val="2083419960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -576,14 +576,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082582504"/>
+        <c:crossAx val="2084307560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2082582504"/>
+        <c:axId val="2084307560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -613,7 +613,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082587272"/>
+        <c:crossAx val="2083419960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -995,7 +995,7 @@
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1200,13 +1200,13 @@
         <v>42</v>
       </c>
       <c r="S4">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="T4">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="U4">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -1262,7 +1262,7 @@
         <v>22</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="S6">
         <v>4</v>
@@ -1336,11 +1336,11 @@
         <v>3</v>
       </c>
       <c r="E12">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F12">
         <f t="shared" ref="F12:F19" si="0">SUM(C12,D12,E12)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="P12" t="s">
         <v>12</v>
@@ -1408,11 +1408,11 @@
         <v>5</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:23">
@@ -1492,11 +1492,11 @@
         <v>2</v>
       </c>
       <c r="E19">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1517,11 +1517,11 @@
       </c>
       <c r="E20">
         <f>SUM(E11:E19)</f>
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="F20">
         <f>SUM(F11:F19)</f>
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
meet with Amee (SM sprint 2)
</commit_message>
<xml_diff>
--- a/bookkeeping/sprint1/overview/s1_burndown.xlsx
+++ b/bookkeeping/sprint1/overview/s1_burndown.xlsx
@@ -521,7 +521,10 @@
                   <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>26.0</c:v>
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -538,11 +541,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2083419960"/>
-        <c:axId val="2084307560"/>
+        <c:axId val="2067206680"/>
+        <c:axId val="2066325704"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2083419960"/>
+        <c:axId val="2067206680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -576,14 +579,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2084307560"/>
+        <c:crossAx val="2066325704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2084307560"/>
+        <c:axId val="2066325704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -613,7 +616,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083419960"/>
+        <c:crossAx val="2067206680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -995,7 +998,7 @@
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1206,7 +1209,10 @@
         <v>28</v>
       </c>
       <c r="U4">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="V4">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -1268,6 +1274,9 @@
         <v>4</v>
       </c>
       <c r="T6">
+        <v>6</v>
+      </c>
+      <c r="U6">
         <v>2</v>
       </c>
     </row>
@@ -1384,11 +1393,11 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="P14" t="s">
         <v>22</v>
@@ -1517,11 +1526,11 @@
       </c>
       <c r="E20">
         <f>SUM(E11:E19)</f>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F20">
         <f>SUM(F11:F19)</f>
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>